<commit_message>
Add usercase description of admin
</commit_message>
<xml_diff>
--- a/02_Document/Usecase/user_cases.xlsx
+++ b/02_Document/Usecase/user_cases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fall2016\CAPSTONE_PROJECT\GitHub\Capstone_ISE0801\02_Document\Usecase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15000" windowHeight="4695"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +53,6 @@
     <t>Choose language</t>
   </si>
   <si>
-    <t>Language opption help visitor easy to use applicaion with selected language and corresponding contents language.</t>
-  </si>
-  <si>
     <t>Free museum</t>
   </si>
   <si>
@@ -69,9 +71,6 @@
     <t>Customer that have an account can login to the system.</t>
   </si>
   <si>
-    <t>Customer that loged in want to logout of system.</t>
-  </si>
-  <si>
     <t>Change customer profile</t>
   </si>
   <si>
@@ -138,12 +137,6 @@
     <t>Change password</t>
   </si>
   <si>
-    <t>Customer that loged in into the system can change their profile.</t>
-  </si>
-  <si>
-    <t>Customer that loged in into the system can change their account's password.</t>
-  </si>
-  <si>
     <t>Customer can upload new objects into system and attach their information.</t>
   </si>
   <si>
@@ -190,6 +183,153 @@
   </si>
   <si>
     <t>Someone who have highest permission on system.</t>
+  </si>
+  <si>
+    <t>UC- 20</t>
+  </si>
+  <si>
+    <t>UC- 21</t>
+  </si>
+  <si>
+    <t>UC- 22</t>
+  </si>
+  <si>
+    <t>UC- 23</t>
+  </si>
+  <si>
+    <t>UC- 24</t>
+  </si>
+  <si>
+    <t>UC- 25</t>
+  </si>
+  <si>
+    <t>UC- 26</t>
+  </si>
+  <si>
+    <t>Admin can login to manages system.</t>
+  </si>
+  <si>
+    <t>Insert new object</t>
+  </si>
+  <si>
+    <t>Need Permission from Museum?</t>
+  </si>
+  <si>
+    <t>Update object's data</t>
+  </si>
+  <si>
+    <t>Delete object</t>
+  </si>
+  <si>
+    <t>Language option help visitor easy to use application with selected language and corresponding contents language.</t>
+  </si>
+  <si>
+    <t>Customer that logged in want to logout of system.</t>
+  </si>
+  <si>
+    <t>Customer that logged in into the system can change their profile.</t>
+  </si>
+  <si>
+    <t>Customer that logged in into the system can change their account's password.</t>
+  </si>
+  <si>
+    <t>Admin that logged in want to logout of system.</t>
+  </si>
+  <si>
+    <t>Admin that logged in into the system can change admin account's password.</t>
+  </si>
+  <si>
+    <t>Admin can change data of exist object in system.</t>
+  </si>
+  <si>
+    <t>Admin can delete exist object in system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept become member request </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reject become member request </t>
+  </si>
+  <si>
+    <t>Answer any comment on every single object</t>
+  </si>
+  <si>
+    <t>Download raw data of object</t>
+  </si>
+  <si>
+    <t>Upload standar data ob project</t>
+  </si>
+  <si>
+    <t>Upload complicated data</t>
+  </si>
+  <si>
+    <t>nên bỏ?</t>
+  </si>
+  <si>
+    <t>UC- 27</t>
+  </si>
+  <si>
+    <t>UC- 28</t>
+  </si>
+  <si>
+    <t>UC- 29</t>
+  </si>
+  <si>
+    <t>Accept request from free museum and create new account for museum</t>
+  </si>
+  <si>
+    <t>Reject request from free museum and notify them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deactivate Museum </t>
+  </si>
+  <si>
+    <t>Activate Museum</t>
+  </si>
+  <si>
+    <t>có nên thêm chức năng deactive/activate data on app</t>
+  </si>
+  <si>
+    <t>Admin can communicate with Museum member through comment on related object .</t>
+  </si>
+  <si>
+    <t>Admin can download raw data uploaded by Museum Member to process and create standar data base on raw data.</t>
+  </si>
+  <si>
+    <t>Admin upload standar data after created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can upload complicated data such as 3D model, </t>
+  </si>
+  <si>
+    <t>Active new Museum's Data</t>
+  </si>
+  <si>
+    <t>Aprove object deleting request</t>
+  </si>
+  <si>
+    <t>Reject object deleting request</t>
+  </si>
+  <si>
+    <t>UC- 30</t>
+  </si>
+  <si>
+    <t>Admin activate standar data after upload</t>
+  </si>
+  <si>
+    <t>Admin has permission to Deactive museum Account</t>
+  </si>
+  <si>
+    <t>Admin has permission to Activate museum Account</t>
+  </si>
+  <si>
+    <t>Admin has permission to insert new object</t>
+  </si>
+  <si>
+    <t>Admin has permission to aprove object deleting request from musemum to delete object from database</t>
+  </si>
+  <si>
+    <t>Admin has permission to reject object deleting request from musemum and still keep object in database.</t>
   </si>
 </sst>
 </file>
@@ -200,7 +340,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -209,7 +349,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -229,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -324,11 +464,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -367,6 +529,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,6 +551,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -424,7 +602,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,7 +637,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,25 +846,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="9.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="46.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.125" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
     <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="30.125" customWidth="1"/>
     <col min="8" max="8" width="43.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -700,9 +878,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -720,9 +898,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -737,12 +915,12 @@
         <v>4</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -751,223 +929,441 @@
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="G5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D14" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D16" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="D17" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
+      <c r="B25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="E24:E25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -979,7 +1375,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -991,7 +1387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>